<commit_message>
clean up ERC, more DFT stuff, started sigma delta adc
</commit_message>
<xml_diff>
--- a/pcb/FPGA-board pinmap.xlsx
+++ b/pcb/FPGA-board pinmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Git_Local\fm_modulator\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD00866-CC18-45E7-8E27-5533F9F00D84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4287657-83AF-422D-9AEE-2C6279405458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13700" yWindow="5670" windowWidth="28800" windowHeight="15560" xr2:uid="{79D2EC7A-782B-4B05-AA36-28D405AEDDBC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
   <si>
     <t>Connector</t>
   </si>
@@ -171,6 +171,9 @@
     <t>k12</t>
   </si>
   <si>
+    <t>c</t>
+  </si>
+  <si>
     <t>DAC_CLK_P</t>
   </si>
   <si>
@@ -208,6 +211,48 @@
   </si>
   <si>
     <t>e9</t>
+  </si>
+  <si>
+    <t>~CW</t>
+  </si>
+  <si>
+    <t>h14</t>
+  </si>
+  <si>
+    <t>CLK_EXT_IN</t>
+  </si>
+  <si>
+    <t>m15</t>
+  </si>
+  <si>
+    <t>h16</t>
+  </si>
+  <si>
+    <t>CLK_OUT</t>
+  </si>
+  <si>
+    <t>LED0</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>LED2</t>
+  </si>
+  <si>
+    <t>LED3</t>
+  </si>
+  <si>
+    <t>f9</t>
+  </si>
+  <si>
+    <t>e8</t>
+  </si>
+  <si>
+    <t>e7</t>
+  </si>
+  <si>
+    <t>d7</t>
   </si>
 </sst>
 </file>
@@ -565,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633A2CA3-C723-4A17-B335-E802AAFF8FDC}">
-  <dimension ref="B5:E33"/>
+  <dimension ref="B5:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -873,86 +918,184 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28">
-        <v>10</v>
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>45</v>
       </c>
       <c r="D28" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C29">
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C30">
         <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C31">
         <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E31" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C32">
         <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C33">
         <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E33" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35">
+        <v>9</v>
+      </c>
+      <c r="D35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37">
+        <v>25</v>
+      </c>
+      <c r="D37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38">
+        <v>19</v>
+      </c>
+      <c r="D38" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40">
+        <v>13</v>
+      </c>
+      <c r="D40" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41">
+        <v>15</v>
+      </c>
+      <c r="D41" t="s">
+        <v>70</v>
+      </c>
+      <c r="E41" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42">
+        <v>17</v>
+      </c>
+      <c r="D42" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43">
+        <v>19</v>
+      </c>
+      <c r="D43" t="s">
+        <v>72</v>
+      </c>
+      <c r="E43" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clean up, label sub circuit blocks in silkscreen document the expected clock and baseband amplitudes based on opamp gains
</commit_message>
<xml_diff>
--- a/pcb/FPGA-board pinmap.xlsx
+++ b/pcb/FPGA-board pinmap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Git_Local\fm_modulator\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4287657-83AF-422D-9AEE-2C6279405458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A5378B-3018-4BAB-9FEC-9605E4B52446}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13700" yWindow="5670" windowWidth="28800" windowHeight="15560" xr2:uid="{79D2EC7A-782B-4B05-AA36-28D405AEDDBC}"/>
+    <workbookView xWindow="-23070" yWindow="2750" windowWidth="28800" windowHeight="15560" xr2:uid="{79D2EC7A-782B-4B05-AA36-28D405AEDDBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
   <si>
     <t>Connector</t>
   </si>
@@ -141,39 +141,6 @@
     <t>B9</t>
   </si>
   <si>
-    <t>g16</t>
-  </si>
-  <si>
-    <t>h15</t>
-  </si>
-  <si>
-    <t>j15</t>
-  </si>
-  <si>
-    <t>k16</t>
-  </si>
-  <si>
-    <t>k14</t>
-  </si>
-  <si>
-    <t>k15</t>
-  </si>
-  <si>
-    <t>l16</t>
-  </si>
-  <si>
-    <t>l14</t>
-  </si>
-  <si>
-    <t>k13</t>
-  </si>
-  <si>
-    <t>k12</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>DAC_CLK_P</t>
   </si>
   <si>
@@ -195,39 +162,12 @@
     <t>J3</t>
   </si>
   <si>
-    <t>d10</t>
-  </si>
-  <si>
-    <t>e10</t>
-  </si>
-  <si>
-    <t>b9</t>
-  </si>
-  <si>
-    <t>a10</t>
-  </si>
-  <si>
-    <t>d8</t>
-  </si>
-  <si>
-    <t>e9</t>
-  </si>
-  <si>
     <t>~CW</t>
   </si>
   <si>
-    <t>h14</t>
-  </si>
-  <si>
     <t>CLK_EXT_IN</t>
   </si>
   <si>
-    <t>m15</t>
-  </si>
-  <si>
-    <t>h16</t>
-  </si>
-  <si>
     <t>CLK_OUT</t>
   </si>
   <si>
@@ -253,6 +193,72 @@
   </si>
   <si>
     <t>d7</t>
+  </si>
+  <si>
+    <t>H15</t>
+  </si>
+  <si>
+    <t>J15</t>
+  </si>
+  <si>
+    <t>K15</t>
+  </si>
+  <si>
+    <t>K16</t>
+  </si>
+  <si>
+    <t>K14</t>
+  </si>
+  <si>
+    <t>L16</t>
+  </si>
+  <si>
+    <t>M16</t>
+  </si>
+  <si>
+    <t>N16</t>
+  </si>
+  <si>
+    <t>L14</t>
+  </si>
+  <si>
+    <t>N14</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>M14</t>
+  </si>
+  <si>
+    <t>H16</t>
+  </si>
+  <si>
+    <t>H14</t>
+  </si>
+  <si>
+    <t>SW0</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>B12</t>
   </si>
 </sst>
 </file>
@@ -610,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633A2CA3-C723-4A17-B335-E802AAFF8FDC}">
-  <dimension ref="B5:E43"/>
+  <dimension ref="B5:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -641,10 +647,10 @@
         <v>24</v>
       </c>
       <c r="C6">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
@@ -655,10 +661,10 @@
         <v>24</v>
       </c>
       <c r="C7">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
@@ -669,10 +675,10 @@
         <v>24</v>
       </c>
       <c r="C8">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -683,10 +689,10 @@
         <v>24</v>
       </c>
       <c r="C9">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -697,10 +703,10 @@
         <v>24</v>
       </c>
       <c r="C10">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -711,10 +717,10 @@
         <v>24</v>
       </c>
       <c r="C11">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -725,10 +731,10 @@
         <v>24</v>
       </c>
       <c r="C12">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -739,10 +745,10 @@
         <v>24</v>
       </c>
       <c r="C13">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -753,10 +759,10 @@
         <v>24</v>
       </c>
       <c r="C14">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -767,10 +773,10 @@
         <v>24</v>
       </c>
       <c r="C15">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
@@ -781,10 +787,10 @@
         <v>24</v>
       </c>
       <c r="C17">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
         <v>25</v>
@@ -795,10 +801,10 @@
         <v>24</v>
       </c>
       <c r="C18">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E18" t="s">
         <v>26</v>
@@ -809,10 +815,10 @@
         <v>24</v>
       </c>
       <c r="C19">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
         <v>20</v>
-      </c>
-      <c r="D19" t="s">
-        <v>37</v>
       </c>
       <c r="E19" t="s">
         <v>27</v>
@@ -823,10 +829,10 @@
         <v>24</v>
       </c>
       <c r="C20">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
         <v>16</v>
-      </c>
-      <c r="D20" t="s">
-        <v>38</v>
       </c>
       <c r="E20" t="s">
         <v>28</v>
@@ -837,10 +843,10 @@
         <v>24</v>
       </c>
       <c r="C21">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
         <v>29</v>
@@ -851,10 +857,10 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="E22" t="s">
         <v>30</v>
@@ -865,10 +871,10 @@
         <v>24</v>
       </c>
       <c r="C23">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="E23" t="s">
         <v>31</v>
@@ -879,10 +885,10 @@
         <v>24</v>
       </c>
       <c r="C24">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="E24" t="s">
         <v>32</v>
@@ -893,10 +899,10 @@
         <v>24</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="E25" t="s">
         <v>33</v>
@@ -907,10 +913,10 @@
         <v>24</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E26" t="s">
         <v>34</v>
@@ -918,86 +924,86 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" t="s">
-        <v>45</v>
+        <v>41</v>
+      </c>
+      <c r="C28">
+        <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="E28" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C29">
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E29" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C30">
         <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="E30" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C31">
         <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E31" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C32">
         <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="E32" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C33">
         <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="E33" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.35">
@@ -1005,97 +1011,125 @@
         <v>24</v>
       </c>
       <c r="C35">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E35" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="C37">
         <v>25</v>
       </c>
       <c r="D37" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E37" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="C38">
         <v>19</v>
       </c>
       <c r="D38" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E38" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C40">
         <v>13</v>
       </c>
       <c r="D40" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="E40" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C41">
         <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="E41" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C42">
         <v>17</v>
       </c>
       <c r="D42" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="E42" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C43">
         <v>19</v>
       </c>
       <c r="D43" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E45" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>74</v>
+      </c>
+      <c r="E46" t="s">
         <v>72</v>
-      </c>
-      <c r="E43" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>